<commit_message>
Managed correctly by reading the badge from the xlsx catalogue
</commit_message>
<xml_diff>
--- a/example_excel/Product list example.xlsx
+++ b/example_excel/Product list example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://almavivaitaliaspa-my.sharepoint.com/personal/a_scarcella_almaviva_it/Documents/Documenti/Excel2PDFCatalog/example_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_EFE1DD3DC9D22D34EC3FC17729A970D378DB3EB3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{835E5A7C-FE4D-488B-8CCB-8D9C822A0B90}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="11_EFE1DD3DC9D22D34EC3FC17729A970D378DB3EB3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76B5FB06-E67A-4228-8F97-C4E6B2D9AFB6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16275" yWindow="1200" windowWidth="30015" windowHeight="15825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="254">
   <si>
     <t>Cat_Merc</t>
   </si>
@@ -96,9 +96,6 @@
     <t>0,33l</t>
   </si>
   <si>
-    <t>Caterory A</t>
-  </si>
-  <si>
     <t>Category B</t>
   </si>
   <si>
@@ -793,6 +790,18 @@
   </si>
   <si>
     <t>Producer 13</t>
+  </si>
+  <si>
+    <t>Badge</t>
+  </si>
+  <si>
+    <t>NEW!</t>
+  </si>
+  <si>
+    <t>Exclusive</t>
+  </si>
+  <si>
+    <t>Category A</t>
   </si>
 </sst>
 </file>
@@ -1106,11 +1115,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1124,7 +1133,7 @@
     <col min="7" max="7" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1146,19 +1155,22 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1167,19 +1179,20 @@
         <v>10.199999999999999</v>
       </c>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -1188,19 +1201,22 @@
         <v>6.5</v>
       </c>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -1209,19 +1225,20 @@
         <v>16</v>
       </c>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
@@ -1230,19 +1247,20 @@
         <v>4.7</v>
       </c>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
@@ -1251,19 +1269,20 @@
         <v>4.7</v>
       </c>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
@@ -1272,19 +1291,20 @@
         <v>3</v>
       </c>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
@@ -1293,19 +1313,20 @@
         <v>5</v>
       </c>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
@@ -1314,19 +1335,20 @@
         <v>1</v>
       </c>
       <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
@@ -1335,19 +1357,20 @@
         <v>1</v>
       </c>
       <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
@@ -1356,19 +1379,22 @@
         <v>1</v>
       </c>
       <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>10</v>
@@ -1377,19 +1403,20 @@
         <v>1.2</v>
       </c>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>11</v>
@@ -1398,19 +1425,20 @@
         <v>0.75</v>
       </c>
       <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>11</v>
@@ -1419,19 +1447,20 @@
         <v>1.5</v>
       </c>
       <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>12</v>
@@ -1440,19 +1469,20 @@
         <v>3</v>
       </c>
       <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>11</v>
@@ -1461,19 +1491,20 @@
         <v>1.5</v>
       </c>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>12</v>
@@ -1482,19 +1513,22 @@
         <v>3</v>
       </c>
       <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>11</v>
@@ -1503,19 +1537,20 @@
         <v>1.5</v>
       </c>
       <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>12</v>
@@ -1524,19 +1559,20 @@
         <v>3</v>
       </c>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>11</v>
@@ -1545,19 +1581,20 @@
         <v>1.5</v>
       </c>
       <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>12</v>
@@ -1566,19 +1603,20 @@
         <v>3</v>
       </c>
       <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>11</v>
@@ -1587,19 +1625,20 @@
         <v>1.5</v>
       </c>
       <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>12</v>
@@ -1608,19 +1647,20 @@
         <v>3</v>
       </c>
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>11</v>
@@ -1629,19 +1669,20 @@
         <v>1.5</v>
       </c>
       <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>12</v>
@@ -1650,19 +1691,22 @@
         <v>3</v>
       </c>
       <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H25" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>11</v>
@@ -1671,19 +1715,20 @@
         <v>1.5</v>
       </c>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>12</v>
@@ -1692,19 +1737,20 @@
         <v>3</v>
       </c>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>11</v>
@@ -1713,19 +1759,20 @@
         <v>1.5</v>
       </c>
       <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>18</v>
+        <v>253</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
@@ -1734,19 +1781,20 @@
         <v>3</v>
       </c>
       <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>11</v>
@@ -1755,19 +1803,20 @@
         <v>1.5</v>
       </c>
       <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>12</v>
@@ -1776,19 +1825,20 @@
         <v>3</v>
       </c>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>17</v>
@@ -1797,19 +1847,20 @@
         <v>2.65</v>
       </c>
       <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>17</v>
@@ -1818,19 +1869,20 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>17</v>
@@ -1839,19 +1891,20 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>17</v>
@@ -1860,19 +1913,20 @@
         <v>2.65</v>
       </c>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
@@ -1881,19 +1935,20 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>17</v>
@@ -1902,19 +1957,20 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1923,19 +1979,20 @@
         <v>2.21</v>
       </c>
       <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>17</v>
@@ -1944,19 +2001,20 @@
         <v>2.35</v>
       </c>
       <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>17</v>
@@ -1965,19 +2023,20 @@
         <v>2.6</v>
       </c>
       <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>13</v>
@@ -1986,19 +2045,20 @@
         <v>1.94</v>
       </c>
       <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>13</v>
@@ -2007,19 +2067,20 @@
         <v>1.94</v>
       </c>
       <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>13</v>
@@ -2028,19 +2089,22 @@
         <v>2.9</v>
       </c>
       <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H43" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>14</v>
@@ -2049,19 +2113,20 @@
         <v>5.95</v>
       </c>
       <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>14</v>
@@ -2070,19 +2135,20 @@
         <v>5.35</v>
       </c>
       <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>13</v>
@@ -2091,19 +2157,20 @@
         <v>2.65</v>
       </c>
       <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>13</v>
@@ -2112,19 +2179,22 @@
         <v>2.9</v>
       </c>
       <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H47" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>14</v>
@@ -2133,19 +2203,20 @@
         <v>5.65</v>
       </c>
       <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>13</v>
@@ -2154,19 +2225,20 @@
         <v>2.8</v>
       </c>
       <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>14</v>
@@ -2175,19 +2247,20 @@
         <v>5.05</v>
       </c>
       <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>13</v>
@@ -2196,19 +2269,20 @@
         <v>2.5</v>
       </c>
       <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>14</v>
@@ -2217,19 +2291,20 @@
         <v>5.55</v>
       </c>
       <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>13</v>
@@ -2238,19 +2313,20 @@
         <v>2.75</v>
       </c>
       <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>14</v>
@@ -2259,19 +2335,20 @@
         <v>4.0928571428571399</v>
       </c>
       <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>13</v>
@@ -2280,19 +2357,22 @@
         <v>4.1732142857142804</v>
       </c>
       <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H55" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>14</v>
@@ -2301,19 +2381,20 @@
         <v>4.2535714285714299</v>
       </c>
       <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>13</v>
@@ -2322,19 +2403,20 @@
         <v>4.3339285714285696</v>
       </c>
       <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>13</v>
@@ -2343,19 +2425,20 @@
         <v>4.4142857142857101</v>
       </c>
       <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>11</v>
@@ -2364,19 +2447,20 @@
         <v>4.4946428571428596</v>
       </c>
       <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>12</v>
@@ -2385,19 +2469,20 @@
         <v>4.5750000000000002</v>
       </c>
       <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H60" s="1"/>
+    </row>
+    <row r="61" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>11</v>
@@ -2406,19 +2491,20 @@
         <v>4.6553571428571399</v>
       </c>
       <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>12</v>
@@ -2427,19 +2513,20 @@
         <v>4.7357142857142902</v>
       </c>
       <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>11</v>
@@ -2448,19 +2535,20 @@
         <v>4.8160714285714299</v>
       </c>
       <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>12</v>
@@ -2469,19 +2557,20 @@
         <v>4.8964285714285696</v>
       </c>
       <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>17</v>
@@ -2490,19 +2579,22 @@
         <v>4.9767857142857101</v>
       </c>
       <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H65" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>8</v>
@@ -2511,19 +2603,20 @@
         <v>5.0571428571428596</v>
       </c>
       <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>9</v>
@@ -2532,19 +2625,20 @@
         <v>5.1375000000000002</v>
       </c>
       <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>10</v>
@@ -2553,61 +2647,66 @@
         <v>5.2178571428571399</v>
       </c>
       <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F69" s="3">
         <v>5.2982142857142902</v>
       </c>
       <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H69" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F70" s="3">
         <v>5.3785714285714299</v>
       </c>
       <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>17</v>
@@ -2616,124 +2715,134 @@
         <v>5.4589285714285696</v>
       </c>
       <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H71" s="1"/>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F72" s="3">
         <v>5.5392857142857101</v>
       </c>
       <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H72" s="1"/>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F73" s="3">
         <v>5.6196428571428596</v>
       </c>
       <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H73" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F74" s="3">
         <v>5.7</v>
       </c>
       <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F75" s="3">
         <v>5.7803571428571399</v>
       </c>
       <c r="G75" s="1"/>
-    </row>
-    <row r="76" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F76" s="3">
         <v>5.8607142857142902</v>
       </c>
       <c r="G76" s="1"/>
-    </row>
-    <row r="77" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H76" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>17</v>
@@ -2742,19 +2851,20 @@
         <v>5.9410714285714299</v>
       </c>
       <c r="G77" s="1"/>
-    </row>
-    <row r="78" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H77" s="1"/>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>15</v>
@@ -2763,103 +2873,108 @@
         <v>6.0214285714285696</v>
       </c>
       <c r="G78" s="1"/>
-    </row>
-    <row r="79" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H78" s="1"/>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F79" s="3">
         <v>6.1017857142857101</v>
       </c>
       <c r="G79" s="1"/>
-    </row>
-    <row r="80" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H79" s="1"/>
+    </row>
+    <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F80" s="3">
         <v>6.1821428571428596</v>
       </c>
       <c r="G80" s="1"/>
-    </row>
-    <row r="81" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H80" s="1"/>
+    </row>
+    <row r="81" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F81" s="3">
         <v>6.2625000000000002</v>
       </c>
       <c r="G81" s="1"/>
-    </row>
-    <row r="82" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H81" s="1"/>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F82" s="3">
         <v>6.3428571428571399</v>
       </c>
       <c r="G82" s="1"/>
-    </row>
-    <row r="83" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H82" s="1"/>
+    </row>
+    <row r="83" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>17</v>
@@ -2868,40 +2983,42 @@
         <v>6.4232142857142902</v>
       </c>
       <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H83" s="1"/>
+    </row>
+    <row r="84" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F84" s="3">
         <v>6.5035714285714299</v>
       </c>
       <c r="G84" s="1"/>
-    </row>
-    <row r="85" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H84" s="1"/>
+    </row>
+    <row r="85" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>16</v>
@@ -2910,82 +3027,88 @@
         <v>6.5839285714285696</v>
       </c>
       <c r="G85" s="1"/>
-    </row>
-    <row r="86" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H85" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F86" s="3">
         <v>6.6642857142857199</v>
       </c>
       <c r="G86" s="1"/>
-    </row>
-    <row r="87" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H86" s="1"/>
+    </row>
+    <row r="87" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F87" s="3">
         <v>6.7446428571428596</v>
       </c>
       <c r="G87" s="1"/>
-    </row>
-    <row r="88" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H87" s="1"/>
+    </row>
+    <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F88" s="3">
         <v>6.8250000000000002</v>
       </c>
       <c r="G88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H88" s="1"/>
+    </row>
+    <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>17</v>
@@ -2994,61 +3117,66 @@
         <v>6.9053571428571399</v>
       </c>
       <c r="G89" s="1"/>
-    </row>
-    <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H89" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F90" s="3">
         <v>6.9857142857142902</v>
       </c>
       <c r="G90" s="1"/>
-    </row>
-    <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H90" s="1"/>
+    </row>
+    <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F91" s="3">
         <v>7.0660714285714299</v>
       </c>
       <c r="G91" s="1"/>
-    </row>
-    <row r="92" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H91" s="1"/>
+    </row>
+    <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>17</v>
@@ -3057,61 +3185,64 @@
         <v>7.1464285714285696</v>
       </c>
       <c r="G92" s="1"/>
-    </row>
-    <row r="93" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H92" s="1"/>
+    </row>
+    <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F93" s="3">
         <v>7.2267857142857199</v>
       </c>
       <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H93" s="1"/>
+    </row>
+    <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F94" s="3">
         <v>7.3071428571428596</v>
       </c>
       <c r="G94" s="1"/>
-    </row>
-    <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H94" s="1"/>
+    </row>
+    <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>10</v>
@@ -3120,61 +3251,66 @@
         <v>7.3875000000000002</v>
       </c>
       <c r="G95" s="1"/>
-    </row>
-    <row r="96" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H95" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F96" s="3">
         <v>7.4678571428571399</v>
       </c>
       <c r="G96" s="1"/>
-    </row>
-    <row r="97" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H96" s="1"/>
+    </row>
+    <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F97" s="3">
         <v>7.5482142857142902</v>
       </c>
       <c r="G97" s="1"/>
-    </row>
-    <row r="98" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H97" s="1"/>
+    </row>
+    <row r="98" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>17</v>
@@ -3183,19 +3319,22 @@
         <v>7.6285714285714299</v>
       </c>
       <c r="G98" s="1"/>
-    </row>
-    <row r="99" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H98" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>15</v>
@@ -3204,54 +3343,57 @@
         <v>7.7089285714285696</v>
       </c>
       <c r="G99" s="1"/>
-    </row>
-    <row r="100" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H99" s="1"/>
+    </row>
+    <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F100" s="3">
         <v>7.7892857142857199</v>
       </c>
       <c r="G100" s="1"/>
-    </row>
-    <row r="101" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H100" s="1"/>
+    </row>
+    <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F101" s="3">
         <v>7.8696428571428596</v>
       </c>
       <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{E30E9127-79F7-452D-AB9E-91F6C97BF535}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="C1:Q706" xr:uid="{685837C6-7B73-4552-8393-D88ABACC57CE}"/>
+      <autoFilter ref="C1:Q706" xr:uid="{DB815519-6C76-4B92-9551-40BA77A0AF6F}"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>